<commit_message>
changed model for planned analysis submission
</commit_message>
<xml_diff>
--- a/model.xlsx
+++ b/model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/injuredroman/Documents/OneDrive/Documents/Senior_Spring_2019/88223/project_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DE1DA05-4F1D-C340-9D4B-CA86CDDB68BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55398C4-6676-E748-9C13-64DD79C895CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2300" yWindow="2800" windowWidth="28040" windowHeight="17440" xr2:uid="{78F6D561-047B-C547-AEEC-659194B8774F}"/>
   </bookViews>
@@ -30,10 +30,81 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="19">
+  <si>
+    <t>Student Willing To Pay</t>
+  </si>
+  <si>
+    <t>For Presentation</t>
+  </si>
+  <si>
+    <t>For Annotated Presentation</t>
+  </si>
+  <si>
+    <t>Amount Willing to Pay for Smartboard:</t>
+  </si>
+  <si>
+    <t>SUM(B2, B3)</t>
+  </si>
+  <si>
+    <t>Amount Willint to Pay for Projector:</t>
+  </si>
+  <si>
+    <t>SUM(B2)</t>
+  </si>
+  <si>
+    <t>Cost to buy Projector:</t>
+  </si>
+  <si>
+    <t>Cost to upkeep Projector, per semester:</t>
+  </si>
+  <si>
+    <t>Cost to buy SMARTBoard:</t>
+  </si>
+  <si>
+    <t>Cost to upkeep SMARTBoard, per semester:</t>
+  </si>
+  <si>
+    <t>Total Cost of SMARTBoard:</t>
+  </si>
+  <si>
+    <t>Total Cost of Projector:</t>
+  </si>
+  <si>
+    <t>SUM(B18, B19)</t>
+  </si>
+  <si>
+    <t>SUM(B14, B15))</t>
+  </si>
+  <si>
+    <t>Sensitivity Analysis on upkeep cost, students willing to pay</t>
+  </si>
+  <si>
+    <t>SMARTBOARD</t>
+  </si>
+  <si>
+    <t>ROW will be Sensitivity on Student's willing to pay --&gt;</t>
+  </si>
+  <si>
+    <t>^ column will be sensitivity to upkeep costs (since initial purchasing cost is well-known/verifiable)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -61,8 +132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,12 +449,328 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276D30B6-0C61-2249-997D-907B76C66600}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>